<commit_message>
Initial id updates but maybe with some extra bits
</commit_message>
<xml_diff>
--- a/source_data/Other/cycles_1.xlsx
+++ b/source_data/Other/cycles_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4C6AD3-FEA0-3D4F-B68F-EA4765A0F395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21EFE91-0638-A64D-9FF9-6ED10A62F49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33440" yWindow="4580" windowWidth="33600" windowHeight="19480" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="33440" yWindow="4580" windowWidth="33600" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="257">
   <si>
     <t>Epoch</t>
   </si>
@@ -898,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -983,6 +983,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2361,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DCDC2E-1983-374F-887E-CD749D9912B4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3086,8 +3089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D034D1-007E-EE43-A36B-40FDFE01FACC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3135,6 +3138,9 @@
       <c r="E2" s="10" t="s">
         <v>96</v>
       </c>
+      <c r="F2" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="G2" s="10" t="s">
         <v>97</v>
       </c>

</xml_diff>